<commit_message>
pcb damn near done
</commit_message>
<xml_diff>
--- a/RESEARCH/parts list.xlsx
+++ b/RESEARCH/parts list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>atmega socket</t>
   </si>
@@ -95,18 +95,9 @@
     <t>10 sockets</t>
   </si>
   <si>
-    <t>opamp</t>
-  </si>
-  <si>
     <t>ask eli</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/LM675T%2FNOPB/LM675T%2FNOPB-ND/32509</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en/connectors-interconnects/terminal-blocks-wire-to-board/1442751</t>
-  </si>
-  <si>
     <t>stockroom</t>
   </si>
   <si>
@@ -174,6 +165,36 @@
   </si>
   <si>
     <t>0805  polarized</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/fairchild-semiconductor/LF353N/LF353NFS-ND/458668</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1-1437664-4/1-1437664-4-ND/2258981</t>
+  </si>
+  <si>
+    <t>500 ohm resistor</t>
+  </si>
+  <si>
+    <t>1200 ohm resistor</t>
+  </si>
+  <si>
+    <t>opamp  4 op amps(2 dips)</t>
+  </si>
+  <si>
+    <t>R1MAP</t>
+  </si>
+  <si>
+    <t>700 ohm resistor</t>
+  </si>
+  <si>
+    <t>R2DIO11/12</t>
+  </si>
+  <si>
+    <t>R2 MAP  / (R1DIO11/12)</t>
+  </si>
+  <si>
+    <t>"0603"</t>
   </si>
 </sst>
 </file>
@@ -502,17 +523,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="6" max="6" width="106.85546875" customWidth="1"/>
   </cols>
@@ -528,7 +549,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -542,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,10 +577,10 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -573,7 +594,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -587,10 +611,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -604,10 +628,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,10 +645,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,7 +676,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,7 +704,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,52 +714,115 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>26</v>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
-        <v>41</v>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +834,9 @@
     <hyperlink ref="F6" r:id="rId5"/>
     <hyperlink ref="F7" r:id="rId6"/>
     <hyperlink ref="F14" r:id="rId7"/>
+    <hyperlink ref="F12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>